<commit_message>
Changed logic for when there are no records.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vodafone-my.sharepoint.com/personal/moneri_mochochoko_vodacom_co_ls/Documents/Documents/UiPath/CourtOrderProcessingREF/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vodafone-my.sharepoint.com/personal/masekate_mokotjo_vodacom_co_ls/Documents/Documents/UiPath/CourtOrderProcessingREF/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="36" documentId="13_ncr:1_{00D541BD-CB78-4D75-8532-9AD73E8C785E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{49C0A847-9140-476F-A9A2-9EEDA485FD88}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1440" yWindow="0" windowWidth="16470" windowHeight="10080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="1" r:id="rId1"/>
@@ -574,16 +574,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="43.5703125" customWidth="1"/>
+    <col min="1" max="1" width="43.54296875" customWidth="1"/>
     <col min="2" max="2" width="43" customWidth="1"/>
-    <col min="3" max="3" width="81.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="81.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -631,7 +631,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="45">
+    <row r="3" spans="1:26" ht="43.5">
       <c r="A3" s="2" t="s">
         <v>30</v>
       </c>
@@ -641,7 +641,7 @@
       </c>
     </row>
     <row r="4" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="5" spans="1:26" ht="30">
+    <row r="5" spans="1:26" ht="29">
       <c r="A5" t="s">
         <v>20</v>
       </c>
@@ -1667,12 +1667,12 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="41" customWidth="1"/>
     <col min="2" max="2" width="51" customWidth="1"/>
-    <col min="3" max="3" width="75.42578125" customWidth="1"/>
-    <col min="4" max="26" width="8.7109375" customWidth="1"/>
+    <col min="3" max="3" width="75.453125" customWidth="1"/>
+    <col min="4" max="26" width="8.7265625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">
@@ -1709,7 +1709,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="30">
+    <row r="2" spans="1:26" ht="29">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -1720,7 +1720,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="45">
+    <row r="3" spans="1:26" ht="43.5">
       <c r="A3" t="s">
         <v>32</v>
       </c>
@@ -1834,7 +1834,7 @@
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="17" spans="1:3" ht="45">
+    <row r="17" spans="1:3" ht="29">
       <c r="A17" t="s">
         <v>39</v>
       </c>
@@ -2826,16 +2826,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Z1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="31.85546875" customWidth="1"/>
-    <col min="2" max="2" width="53.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="60.28515625" customWidth="1"/>
-    <col min="4" max="26" width="65.42578125" customWidth="1"/>
+    <col min="1" max="1" width="31.81640625" customWidth="1"/>
+    <col min="2" max="2" width="53.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="60.26953125" customWidth="1"/>
+    <col min="4" max="26" width="65.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="14.25" customHeight="1">

</xml_diff>